<commit_message>
Update code and tests for arms and epochs
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/annotations_and_abbreviations.xlsx
+++ b/tests/integration_test_files/annotations_and_abbreviations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08972F1F-F2C4-C441-A330-F3609729866E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D72E7DB-4343-5E4B-A5DD-075334B2C4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41460" yWindow="2980" windowWidth="58640" windowHeight="23700" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47680" yWindow="2980" windowWidth="52420" windowHeight="23700" firstSheet="11" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3302" uniqueCount="1246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3308" uniqueCount="1249">
   <si>
     <t>name</t>
   </si>
@@ -3808,6 +3808,15 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t>ANN_01, ANN_04</t>
+  </si>
+  <si>
+    <t>ANN_04</t>
+  </si>
+  <si>
+    <t>Additional note</t>
   </si>
 </sst>
 </file>
@@ -6028,7 +6037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -10624,10 +10633,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFABB680-8BAD-E04C-BA6A-5C36BD53129A}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10668,6 +10677,14 @@
       </c>
       <c r="B4" t="s">
         <v>1244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1248</v>
       </c>
     </row>
   </sheetData>
@@ -14608,10 +14625,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14621,9 +14638,10 @@
     <col min="4" max="4" width="23.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="32.1640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="25.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -14642,8 +14660,11 @@
       <c r="F1" s="21" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G1" s="21" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
         <v>128</v>
       </c>
@@ -14662,8 +14683,11 @@
       <c r="F2" s="3" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="3" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>97</v>
       </c>
@@ -14683,7 +14707,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>99</v>
       </c>
@@ -14710,10 +14734,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14724,7 +14748,7 @@
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -14737,8 +14761,11 @@
       <c r="D1" s="21" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="21" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>134</v>
       </c>
@@ -14751,8 +14778,11 @@
       <c r="D2" s="3" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="3" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>89</v>
       </c>
@@ -14766,7 +14796,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>90</v>
       </c>
@@ -14780,7 +14810,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>91</v>
       </c>
@@ -14794,7 +14824,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
Add macro and tests
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/annotations_and_abbreviations.xlsx
+++ b/tests/integration_test_files/annotations_and_abbreviations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D72E7DB-4343-5E4B-A5DD-075334B2C4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9E1B11-9AA5-CB45-A1A1-5C34B8550602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47680" yWindow="2980" windowWidth="52420" windowHeight="23700" firstSheet="11" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50280" yWindow="2760" windowWidth="52420" windowHeight="23700" firstSheet="12" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -38,16 +38,17 @@
     <sheet name="dictionaries" sheetId="23" r:id="rId23"/>
     <sheet name="somethingElse" sheetId="24" r:id="rId24"/>
     <sheet name="annotations" sheetId="28" r:id="rId25"/>
-    <sheet name="spareFormat" sheetId="25" r:id="rId26"/>
-    <sheet name="configuration" sheetId="26" r:id="rId27"/>
-    <sheet name="documentContent" sheetId="27" r:id="rId28"/>
+    <sheet name="abbreviations" sheetId="29" r:id="rId26"/>
+    <sheet name="spareFormat" sheetId="25" r:id="rId27"/>
+    <sheet name="configuration" sheetId="26" r:id="rId28"/>
+    <sheet name="documentContent" sheetId="27" r:id="rId29"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3308" uniqueCount="1249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3313" uniqueCount="1252">
   <si>
     <t>name</t>
   </si>
@@ -3817,6 +3818,15 @@
   </si>
   <si>
     <t>Additional note</t>
+  </si>
+  <si>
+    <t>abbreviatedText</t>
+  </si>
+  <si>
+    <t>expandedText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electrocardiogram </t>
   </si>
 </sst>
 </file>
@@ -10635,7 +10645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFABB680-8BAD-E04C-BA6A-5C36BD53129A}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -10693,6 +10703,44 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05D5AB3-28F9-594C-AE35-2D8023E05070}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="52" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:F133"/>
   <sheetViews>
@@ -13375,7 +13423,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -13451,12 +13499,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{250E6F23-B764-5243-842F-046C5535819A}">
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView topLeftCell="A122" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A133" sqref="A2:A133"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>